<commit_message>
Added script to fetch lichess games
</commit_message>
<xml_diff>
--- a/chesstempo_tactics.xlsx
+++ b/chesstempo_tactics.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="828" uniqueCount="543">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1080" uniqueCount="704">
   <si>
     <t>969.4</t>
   </si>
@@ -1653,6 +1653,489 @@
   </si>
   <si>
     <t>1328.3 (+1.9)</t>
+  </si>
+  <si>
+    <t>1179.3</t>
+  </si>
+  <si>
+    <t>1335.1 (+2.0)</t>
+  </si>
+  <si>
+    <t>1242.4</t>
+  </si>
+  <si>
+    <t>1333.1 (+2.6)</t>
+  </si>
+  <si>
+    <t>1226.4</t>
+  </si>
+  <si>
+    <t>1330.5 (+2.5)</t>
+  </si>
+  <si>
+    <t>1196.1</t>
+  </si>
+  <si>
+    <t>1328.0 (+2.2)</t>
+  </si>
+  <si>
+    <t>1325.7 (+2.6)</t>
+  </si>
+  <si>
+    <t>1265.0</t>
+  </si>
+  <si>
+    <t>1323.1 (+2.9)</t>
+  </si>
+  <si>
+    <t>1183.1</t>
+  </si>
+  <si>
+    <t>1320.2 (+2.2)</t>
+  </si>
+  <si>
+    <t>1083.8</t>
+  </si>
+  <si>
+    <t>1318.0 (+1.5)</t>
+  </si>
+  <si>
+    <t>1316.6 (-4.5)</t>
+  </si>
+  <si>
+    <t>1134.5</t>
+  </si>
+  <si>
+    <t>1321.0 (+1.8)</t>
+  </si>
+  <si>
+    <t>1193.9</t>
+  </si>
+  <si>
+    <t>1319.2 (-4.7)</t>
+  </si>
+  <si>
+    <t>1439.9</t>
+  </si>
+  <si>
+    <t>1324.0 (-2.4)</t>
+  </si>
+  <si>
+    <t>1277.7</t>
+  </si>
+  <si>
+    <t>1326.4 (+3.1)</t>
+  </si>
+  <si>
+    <t>1268.3</t>
+  </si>
+  <si>
+    <t>1323.3 (-4.3)</t>
+  </si>
+  <si>
+    <t>1317.1</t>
+  </si>
+  <si>
+    <t>1338.0 (-3.7)</t>
+  </si>
+  <si>
+    <t>1213.4</t>
+  </si>
+  <si>
+    <t>1341.7 (+2.3)</t>
+  </si>
+  <si>
+    <t>1151.8</t>
+  </si>
+  <si>
+    <t>1339.4 (-5.3)</t>
+  </si>
+  <si>
+    <t>1317.3</t>
+  </si>
+  <si>
+    <t>1344.7 (+3.2)</t>
+  </si>
+  <si>
+    <t>1306.5</t>
+  </si>
+  <si>
+    <t>1341.5 (+3.2)</t>
+  </si>
+  <si>
+    <t>1258.5</t>
+  </si>
+  <si>
+    <t>1338.3 (+2.7)</t>
+  </si>
+  <si>
+    <t>1098.4</t>
+  </si>
+  <si>
+    <t>1335.6 (+1.4)</t>
+  </si>
+  <si>
+    <t>1296.8</t>
+  </si>
+  <si>
+    <t>1334.1 (-3.9)</t>
+  </si>
+  <si>
+    <t>1275.2</t>
+  </si>
+  <si>
+    <t>1338.0 (+2.9)</t>
+  </si>
+  <si>
+    <t>1137.3</t>
+  </si>
+  <si>
+    <t>1358.7 (+1.5)</t>
+  </si>
+  <si>
+    <t>1166.6</t>
+  </si>
+  <si>
+    <t>1357.2 (-5.3)</t>
+  </si>
+  <si>
+    <t>1433.5</t>
+  </si>
+  <si>
+    <t>1362.5 (+4.2)</t>
+  </si>
+  <si>
+    <t>1137.1</t>
+  </si>
+  <si>
+    <t>1358.2 (+1.5)</t>
+  </si>
+  <si>
+    <t>1277.6</t>
+  </si>
+  <si>
+    <t>1356.7 (+2.7)</t>
+  </si>
+  <si>
+    <t>1104.5</t>
+  </si>
+  <si>
+    <t>1354.0 (+1.4)</t>
+  </si>
+  <si>
+    <t>1191.0</t>
+  </si>
+  <si>
+    <t>1352.6 (+2.0)</t>
+  </si>
+  <si>
+    <t>1228.9</t>
+  </si>
+  <si>
+    <t>1350.6 (+2.3)</t>
+  </si>
+  <si>
+    <t>1063.7</t>
+  </si>
+  <si>
+    <t>1348.3 (+1.1)</t>
+  </si>
+  <si>
+    <t>1404.1</t>
+  </si>
+  <si>
+    <t>1347.1 (+4.1)</t>
+  </si>
+  <si>
+    <t>1273.9</t>
+  </si>
+  <si>
+    <t>1343.0 (+2.8)</t>
+  </si>
+  <si>
+    <t>1204.9</t>
+  </si>
+  <si>
+    <t>1340.2 (+2.2)</t>
+  </si>
+  <si>
+    <t>1379.6</t>
+  </si>
+  <si>
+    <t>1350.8 (-3.2)</t>
+  </si>
+  <si>
+    <t>1354.1 (-4.8)</t>
+  </si>
+  <si>
+    <t>1283.3</t>
+  </si>
+  <si>
+    <t>1358.9 (+2.8)</t>
+  </si>
+  <si>
+    <t>1173.5</t>
+  </si>
+  <si>
+    <t>1356.1 (-5.2)</t>
+  </si>
+  <si>
+    <t>1232.7</t>
+  </si>
+  <si>
+    <t>1361.3 (+2.3)</t>
+  </si>
+  <si>
+    <t>1297.7</t>
+  </si>
+  <si>
+    <t>1359.1 (+2.9)</t>
+  </si>
+  <si>
+    <t>1356.1 (+2.0)</t>
+  </si>
+  <si>
+    <t>1284.1</t>
+  </si>
+  <si>
+    <t>1354.1 (-4.2)</t>
+  </si>
+  <si>
+    <t>1087.0</t>
+  </si>
+  <si>
+    <t>1358.3 (+1.2)</t>
+  </si>
+  <si>
+    <t>1004.7</t>
+  </si>
+  <si>
+    <t>1357.1 (+0.8)</t>
+  </si>
+  <si>
+    <t>1165.0</t>
+  </si>
+  <si>
+    <t>1356.3 (-5.3)</t>
+  </si>
+  <si>
+    <t>1278.2</t>
+  </si>
+  <si>
+    <t>1361.6 (+2.7)</t>
+  </si>
+  <si>
+    <t>1316.5</t>
+  </si>
+  <si>
+    <t>1358.9 (+3.1)</t>
+  </si>
+  <si>
+    <t>1059.6</t>
+  </si>
+  <si>
+    <t>1355.8 (+1.1)</t>
+  </si>
+  <si>
+    <t>1306.0</t>
+  </si>
+  <si>
+    <t>1354.7 (-4.0)</t>
+  </si>
+  <si>
+    <t>1379.2</t>
+  </si>
+  <si>
+    <t>1349.7 (+3.8)</t>
+  </si>
+  <si>
+    <t>1200.8</t>
+  </si>
+  <si>
+    <t>1345.9 (+2.1)</t>
+  </si>
+  <si>
+    <t>1283.0</t>
+  </si>
+  <si>
+    <t>1343.8 (+2.9)</t>
+  </si>
+  <si>
+    <t>1111.3</t>
+  </si>
+  <si>
+    <t>1340.9 (-5.6)</t>
+  </si>
+  <si>
+    <t>1132.2</t>
+  </si>
+  <si>
+    <t>1346.4 (+1.6)</t>
+  </si>
+  <si>
+    <t>1266.5</t>
+  </si>
+  <si>
+    <t>1344.9 (-4.3)</t>
+  </si>
+  <si>
+    <t>1259.6</t>
+  </si>
+  <si>
+    <t>1349.2 (-4.4)</t>
+  </si>
+  <si>
+    <t>1236.1</t>
+  </si>
+  <si>
+    <t>1353.6 (+2.4)</t>
+  </si>
+  <si>
+    <t>1163.7</t>
+  </si>
+  <si>
+    <t>1351.2 (+1.8)</t>
+  </si>
+  <si>
+    <t>1308.9</t>
+  </si>
+  <si>
+    <t>1349.4 (-3.9)</t>
+  </si>
+  <si>
+    <t>1249.4</t>
+  </si>
+  <si>
+    <t>1353.3 (+2.5)</t>
+  </si>
+  <si>
+    <t>1295.0</t>
+  </si>
+  <si>
+    <t>1376.5 (+2.7)</t>
+  </si>
+  <si>
+    <t>1225.9</t>
+  </si>
+  <si>
+    <t>1373.8 (+2.1)</t>
+  </si>
+  <si>
+    <t>1290.8</t>
+  </si>
+  <si>
+    <t>1371.7 (+2.7)</t>
+  </si>
+  <si>
+    <t>1266.4</t>
+  </si>
+  <si>
+    <t>1369.0 (+2.5)</t>
+  </si>
+  <si>
+    <t>1299.5</t>
+  </si>
+  <si>
+    <t>1366.5 (+2.9)</t>
+  </si>
+  <si>
+    <t>1258.0</t>
+  </si>
+  <si>
+    <t>1363.6 (+2.5)</t>
+  </si>
+  <si>
+    <t>1279.7</t>
+  </si>
+  <si>
+    <t>1361.2 (-4.3)</t>
+  </si>
+  <si>
+    <t>1212.0</t>
+  </si>
+  <si>
+    <t>1365.5 (+2.1)</t>
+  </si>
+  <si>
+    <t>1294.5</t>
+  </si>
+  <si>
+    <t>1363.4 (+2.8)</t>
+  </si>
+  <si>
+    <t>1349.7</t>
+  </si>
+  <si>
+    <t>1360.6 (+3.4)</t>
+  </si>
+  <si>
+    <t>1010.0</t>
+  </si>
+  <si>
+    <t>1357.2 (+0.8)</t>
+  </si>
+  <si>
+    <t>1356.3 (+2.0)</t>
+  </si>
+  <si>
+    <t>1226.5</t>
+  </si>
+  <si>
+    <t>1354.3 (-4.8)</t>
+  </si>
+  <si>
+    <t>1009.7</t>
+  </si>
+  <si>
+    <t>1359.1 (+0.8)</t>
+  </si>
+  <si>
+    <t>1279.4</t>
+  </si>
+  <si>
+    <t>1358.3 (-4.3)</t>
+  </si>
+  <si>
+    <t>1239.6</t>
+  </si>
+  <si>
+    <t>1362.6 (+2.3)</t>
+  </si>
+  <si>
+    <t>1151.4</t>
+  </si>
+  <si>
+    <t>1360.2 (+1.6)</t>
+  </si>
+  <si>
+    <t>1358.6 (+2.6)</t>
+  </si>
+  <si>
+    <t>1218.1</t>
+  </si>
+  <si>
+    <t>1356.0 (-4.9)</t>
+  </si>
+  <si>
+    <t>1424.5</t>
+  </si>
+  <si>
+    <t>1360.9 (+4.2)</t>
+  </si>
+  <si>
+    <t>1205.2</t>
+  </si>
+  <si>
+    <t>1356.7 (+2.1)</t>
+  </si>
+  <si>
+    <t>1354.6 (+2.2)</t>
+  </si>
+  <si>
+    <t>1269.0</t>
+  </si>
+  <si>
+    <t>1352.4 (+2.7)</t>
   </si>
 </sst>
 </file>
@@ -1972,10 +2455,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I274"/>
+  <dimension ref="A1:I358"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A260" workbookViewId="0">
-      <selection activeCell="A265" sqref="A265:I274"/>
+    <sheetView tabSelected="1" topLeftCell="A335" workbookViewId="0">
+      <selection activeCell="J336" sqref="J336"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9929,6 +10412,2442 @@
         <v>542</v>
       </c>
     </row>
+    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A275">
+        <v>1</v>
+      </c>
+      <c r="B275" s="1">
+        <v>42739.484444444446</v>
+      </c>
+      <c r="C275">
+        <v>28367</v>
+      </c>
+      <c r="D275" t="s">
+        <v>543</v>
+      </c>
+      <c r="E275" t="s">
+        <v>1</v>
+      </c>
+      <c r="F275" s="2">
+        <v>2.9861111111111113E-2</v>
+      </c>
+      <c r="G275" s="2">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="H275" s="2">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="I275" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A276">
+        <v>2</v>
+      </c>
+      <c r="B276" s="1">
+        <v>42739.48400462963</v>
+      </c>
+      <c r="C276">
+        <v>60646</v>
+      </c>
+      <c r="D276" t="s">
+        <v>545</v>
+      </c>
+      <c r="E276" t="s">
+        <v>1</v>
+      </c>
+      <c r="F276" s="2">
+        <v>6.1111111111111116E-2</v>
+      </c>
+      <c r="G276" s="2">
+        <v>2.2222222222222223E-2</v>
+      </c>
+      <c r="H276" s="2">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="I276" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A277">
+        <v>3</v>
+      </c>
+      <c r="B277" s="1">
+        <v>42739.483587962961</v>
+      </c>
+      <c r="C277">
+        <v>40465</v>
+      </c>
+      <c r="D277" t="s">
+        <v>547</v>
+      </c>
+      <c r="E277" t="s">
+        <v>1</v>
+      </c>
+      <c r="F277" s="2">
+        <v>4.7916666666666663E-2</v>
+      </c>
+      <c r="G277" s="2">
+        <v>1.1805555555555555E-2</v>
+      </c>
+      <c r="H277" s="2">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="I277" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A278">
+        <v>4</v>
+      </c>
+      <c r="B278" s="1">
+        <v>42739.483356481483</v>
+      </c>
+      <c r="C278">
+        <v>14013</v>
+      </c>
+      <c r="D278" t="s">
+        <v>549</v>
+      </c>
+      <c r="E278" t="s">
+        <v>1</v>
+      </c>
+      <c r="F278" s="2">
+        <v>4.6527777777777779E-2</v>
+      </c>
+      <c r="G278" s="2">
+        <v>3.0555555555555555E-2</v>
+      </c>
+      <c r="H278" s="2">
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="I278" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A279">
+        <v>5</v>
+      </c>
+      <c r="B279" s="1">
+        <v>42739.482800925929</v>
+      </c>
+      <c r="C279">
+        <v>76593</v>
+      </c>
+      <c r="D279" t="s">
+        <v>220</v>
+      </c>
+      <c r="E279" t="s">
+        <v>1</v>
+      </c>
+      <c r="F279" s="2">
+        <v>5.2777777777777778E-2</v>
+      </c>
+      <c r="G279" s="2">
+        <v>2.9166666666666664E-2</v>
+      </c>
+      <c r="H279" s="2">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="I279" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="280" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A280">
+        <v>6</v>
+      </c>
+      <c r="B280" s="1">
+        <v>42739.482256944444</v>
+      </c>
+      <c r="C280">
+        <v>15297</v>
+      </c>
+      <c r="D280" t="s">
+        <v>552</v>
+      </c>
+      <c r="E280" t="s">
+        <v>1</v>
+      </c>
+      <c r="F280" s="2">
+        <v>5.2777777777777778E-2</v>
+      </c>
+      <c r="G280" s="2">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="H280" s="2">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="I280" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A281">
+        <v>7</v>
+      </c>
+      <c r="B281" s="1">
+        <v>42739.481585648151</v>
+      </c>
+      <c r="C281">
+        <v>23034</v>
+      </c>
+      <c r="D281" t="s">
+        <v>554</v>
+      </c>
+      <c r="E281" t="s">
+        <v>1</v>
+      </c>
+      <c r="F281" s="2">
+        <v>5.486111111111111E-2</v>
+      </c>
+      <c r="G281" s="2">
+        <v>0.12222222222222223</v>
+      </c>
+      <c r="H281" s="2">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="I281" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="282" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A282">
+        <v>8</v>
+      </c>
+      <c r="B282" s="1">
+        <v>42739.479502314818</v>
+      </c>
+      <c r="C282">
+        <v>50818</v>
+      </c>
+      <c r="D282" t="s">
+        <v>556</v>
+      </c>
+      <c r="E282" t="s">
+        <v>1</v>
+      </c>
+      <c r="F282" s="2">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="G282" s="2">
+        <v>9.0277777777777787E-3</v>
+      </c>
+      <c r="H282" s="2">
+        <v>0</v>
+      </c>
+      <c r="I282" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="283" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A283">
+        <v>9</v>
+      </c>
+      <c r="B283" s="1">
+        <v>42739.479120370372</v>
+      </c>
+      <c r="C283">
+        <v>174631</v>
+      </c>
+      <c r="D283" t="s">
+        <v>374</v>
+      </c>
+      <c r="E283" t="s">
+        <v>1</v>
+      </c>
+      <c r="F283" s="2">
+        <v>7.7777777777777779E-2</v>
+      </c>
+      <c r="G283" s="2">
+        <v>0.12013888888888889</v>
+      </c>
+      <c r="H283" s="2">
+        <v>0</v>
+      </c>
+      <c r="I283" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="284" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A284">
+        <v>10</v>
+      </c>
+      <c r="B284" s="1">
+        <v>42739.477071759262</v>
+      </c>
+      <c r="C284">
+        <v>88448</v>
+      </c>
+      <c r="D284" t="s">
+        <v>559</v>
+      </c>
+      <c r="E284" t="s">
+        <v>1</v>
+      </c>
+      <c r="F284" s="2">
+        <v>4.3055555555555562E-2</v>
+      </c>
+      <c r="G284" s="2">
+        <v>1.3194444444444444E-2</v>
+      </c>
+      <c r="H284" s="2">
+        <v>2.7777777777777779E-3</v>
+      </c>
+      <c r="I284" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="285" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A285">
+        <v>11</v>
+      </c>
+      <c r="B285" s="1">
+        <v>42739.4766087963</v>
+      </c>
+      <c r="C285">
+        <v>52953</v>
+      </c>
+      <c r="D285" t="s">
+        <v>561</v>
+      </c>
+      <c r="E285" t="s">
+        <v>1</v>
+      </c>
+      <c r="F285" s="2">
+        <v>2.1527777777777781E-2</v>
+      </c>
+      <c r="G285" s="2">
+        <v>9.0277777777777787E-3</v>
+      </c>
+      <c r="H285" s="2">
+        <v>0</v>
+      </c>
+      <c r="I285" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="286" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A286">
+        <v>12</v>
+      </c>
+      <c r="B286" s="1">
+        <v>42739.476157407407</v>
+      </c>
+      <c r="C286">
+        <v>103694</v>
+      </c>
+      <c r="D286" t="s">
+        <v>563</v>
+      </c>
+      <c r="E286" t="s">
+        <v>1</v>
+      </c>
+      <c r="F286" s="2">
+        <v>9.5138888888888884E-2</v>
+      </c>
+      <c r="G286" s="2">
+        <v>9.375E-2</v>
+      </c>
+      <c r="H286" s="2">
+        <v>0</v>
+      </c>
+      <c r="I286" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="287" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A287">
+        <v>13</v>
+      </c>
+      <c r="B287" s="1">
+        <v>42739.474537037036</v>
+      </c>
+      <c r="C287">
+        <v>61740</v>
+      </c>
+      <c r="D287" t="s">
+        <v>565</v>
+      </c>
+      <c r="E287" t="s">
+        <v>1</v>
+      </c>
+      <c r="F287" s="2">
+        <v>9.1666666666666674E-2</v>
+      </c>
+      <c r="G287" s="2">
+        <v>5.7638888888888885E-2</v>
+      </c>
+      <c r="H287" s="2">
+        <v>4.8611111111111112E-3</v>
+      </c>
+      <c r="I287" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="288" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A288">
+        <v>14</v>
+      </c>
+      <c r="B288" s="1">
+        <v>42739.473437499997</v>
+      </c>
+      <c r="C288">
+        <v>98210</v>
+      </c>
+      <c r="D288" t="s">
+        <v>567</v>
+      </c>
+      <c r="E288" t="s">
+        <v>1</v>
+      </c>
+      <c r="F288" s="2">
+        <v>7.013888888888889E-2</v>
+      </c>
+      <c r="G288" s="2">
+        <v>3.7499999999999999E-2</v>
+      </c>
+      <c r="H288" s="2">
+        <v>0</v>
+      </c>
+      <c r="I288" t="s">
+        <v>568</v>
+      </c>
+    </row>
+    <row r="289" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A289">
+        <v>1</v>
+      </c>
+      <c r="B289" s="1">
+        <v>42739.509953703702</v>
+      </c>
+      <c r="C289">
+        <v>177721</v>
+      </c>
+      <c r="D289" t="s">
+        <v>569</v>
+      </c>
+      <c r="E289" t="s">
+        <v>1</v>
+      </c>
+      <c r="F289" s="2">
+        <v>0.12986111111111112</v>
+      </c>
+      <c r="G289" s="2">
+        <v>5.347222222222222E-2</v>
+      </c>
+      <c r="H289" s="2">
+        <v>0</v>
+      </c>
+      <c r="I289" t="s">
+        <v>570</v>
+      </c>
+    </row>
+    <row r="290" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A290">
+        <v>2</v>
+      </c>
+      <c r="B290" s="1">
+        <v>42739.509016203701</v>
+      </c>
+      <c r="C290">
+        <v>102911</v>
+      </c>
+      <c r="D290" t="s">
+        <v>571</v>
+      </c>
+      <c r="E290" t="s">
+        <v>1</v>
+      </c>
+      <c r="F290" s="2">
+        <v>0.10069444444444443</v>
+      </c>
+      <c r="G290" s="2">
+        <v>0.26041666666666669</v>
+      </c>
+      <c r="H290" s="2">
+        <v>1.1111111111111112E-2</v>
+      </c>
+      <c r="I290" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="291" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A291">
+        <v>3</v>
+      </c>
+      <c r="B291" s="1">
+        <v>42739.504467592589</v>
+      </c>
+      <c r="C291">
+        <v>78868</v>
+      </c>
+      <c r="D291" t="s">
+        <v>573</v>
+      </c>
+      <c r="E291" t="s">
+        <v>1</v>
+      </c>
+      <c r="F291" s="2">
+        <v>5.9722222222222225E-2</v>
+      </c>
+      <c r="G291" s="2">
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="H291" s="2">
+        <v>0</v>
+      </c>
+      <c r="I291" t="s">
+        <v>574</v>
+      </c>
+    </row>
+    <row r="292" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A292">
+        <v>4</v>
+      </c>
+      <c r="B292" s="1">
+        <v>42739.504282407404</v>
+      </c>
+      <c r="C292">
+        <v>73288</v>
+      </c>
+      <c r="D292" t="s">
+        <v>575</v>
+      </c>
+      <c r="E292" t="s">
+        <v>1</v>
+      </c>
+      <c r="F292" s="2">
+        <v>7.2222222222222229E-2</v>
+      </c>
+      <c r="G292" s="2">
+        <v>3.6111111111111115E-2</v>
+      </c>
+      <c r="H292" s="2">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="I292" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="293" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A293">
+        <v>5</v>
+      </c>
+      <c r="B293" s="1">
+        <v>42739.503634259258</v>
+      </c>
+      <c r="C293">
+        <v>115765</v>
+      </c>
+      <c r="D293" t="s">
+        <v>577</v>
+      </c>
+      <c r="E293" t="s">
+        <v>1</v>
+      </c>
+      <c r="F293" s="2">
+        <v>6.9444444444444434E-2</v>
+      </c>
+      <c r="G293" s="2">
+        <v>2.2916666666666669E-2</v>
+      </c>
+      <c r="H293" s="2">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="I293" t="s">
+        <v>578</v>
+      </c>
+    </row>
+    <row r="294" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A294">
+        <v>6</v>
+      </c>
+      <c r="B294" s="1">
+        <v>42739.503194444442</v>
+      </c>
+      <c r="C294">
+        <v>21662</v>
+      </c>
+      <c r="D294" t="s">
+        <v>579</v>
+      </c>
+      <c r="E294" t="s">
+        <v>1</v>
+      </c>
+      <c r="F294" s="2">
+        <v>5.347222222222222E-2</v>
+      </c>
+      <c r="G294" s="2">
+        <v>1.1111111111111112E-2</v>
+      </c>
+      <c r="H294" s="2">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="I294" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="295" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A295">
+        <v>7</v>
+      </c>
+      <c r="B295" s="1">
+        <v>42739.502962962964</v>
+      </c>
+      <c r="C295">
+        <v>70933</v>
+      </c>
+      <c r="D295" t="s">
+        <v>581</v>
+      </c>
+      <c r="E295" t="s">
+        <v>1</v>
+      </c>
+      <c r="F295" s="2">
+        <v>4.9999999999999996E-2</v>
+      </c>
+      <c r="G295" s="2">
+        <v>2.5694444444444447E-2</v>
+      </c>
+      <c r="H295" s="2">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="I295" t="s">
+        <v>582</v>
+      </c>
+    </row>
+    <row r="296" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A296">
+        <v>8</v>
+      </c>
+      <c r="B296" s="1">
+        <v>42739.502060185187</v>
+      </c>
+      <c r="C296">
+        <v>78005</v>
+      </c>
+      <c r="D296" t="s">
+        <v>583</v>
+      </c>
+      <c r="E296" t="s">
+        <v>1</v>
+      </c>
+      <c r="F296" s="2">
+        <v>8.4722222222222213E-2</v>
+      </c>
+      <c r="G296" s="2">
+        <v>0.15972222222222224</v>
+      </c>
+      <c r="H296" s="2">
+        <v>0</v>
+      </c>
+      <c r="I296" t="s">
+        <v>584</v>
+      </c>
+    </row>
+    <row r="297" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A297">
+        <v>9</v>
+      </c>
+      <c r="B297" s="1">
+        <v>42739.499363425923</v>
+      </c>
+      <c r="C297">
+        <v>159166</v>
+      </c>
+      <c r="D297" t="s">
+        <v>585</v>
+      </c>
+      <c r="E297" t="s">
+        <v>1</v>
+      </c>
+      <c r="F297" s="2">
+        <v>7.7777777777777779E-2</v>
+      </c>
+      <c r="G297" s="2">
+        <v>2.6388888888888889E-2</v>
+      </c>
+      <c r="H297" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="I297" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="298" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A298">
+        <v>1</v>
+      </c>
+      <c r="B298" s="1">
+        <v>42739.536585648151</v>
+      </c>
+      <c r="C298">
+        <v>55374</v>
+      </c>
+      <c r="D298" t="s">
+        <v>587</v>
+      </c>
+      <c r="E298" t="s">
+        <v>1</v>
+      </c>
+      <c r="F298" s="2">
+        <v>4.2361111111111106E-2</v>
+      </c>
+      <c r="G298" s="2">
+        <v>1.1111111111111112E-2</v>
+      </c>
+      <c r="H298" s="2">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="I298" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="299" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A299">
+        <v>2</v>
+      </c>
+      <c r="B299" s="1">
+        <v>42739.535196759258</v>
+      </c>
+      <c r="C299">
+        <v>18170</v>
+      </c>
+      <c r="D299" t="s">
+        <v>589</v>
+      </c>
+      <c r="E299" t="s">
+        <v>1</v>
+      </c>
+      <c r="F299" s="2">
+        <v>4.3750000000000004E-2</v>
+      </c>
+      <c r="G299" s="2">
+        <v>8.1250000000000003E-2</v>
+      </c>
+      <c r="H299" s="2">
+        <v>0</v>
+      </c>
+      <c r="I299" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="300" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A300">
+        <v>3</v>
+      </c>
+      <c r="B300" s="1">
+        <v>42739.533622685187</v>
+      </c>
+      <c r="C300">
+        <v>75617</v>
+      </c>
+      <c r="D300" t="s">
+        <v>591</v>
+      </c>
+      <c r="E300" t="s">
+        <v>1</v>
+      </c>
+      <c r="F300" s="2">
+        <v>5.1388888888888894E-2</v>
+      </c>
+      <c r="G300" s="2">
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="H300" s="2">
+        <v>2.7777777777777779E-3</v>
+      </c>
+      <c r="I300" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="301" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A301">
+        <v>4</v>
+      </c>
+      <c r="B301" s="1">
+        <v>42739.533182870371</v>
+      </c>
+      <c r="C301">
+        <v>156689</v>
+      </c>
+      <c r="D301" t="s">
+        <v>593</v>
+      </c>
+      <c r="E301" t="s">
+        <v>1</v>
+      </c>
+      <c r="F301" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="G301" s="2">
+        <v>9.7222222222222224E-3</v>
+      </c>
+      <c r="H301" s="2">
+        <v>2.7777777777777779E-3</v>
+      </c>
+      <c r="I301" t="s">
+        <v>594</v>
+      </c>
+    </row>
+    <row r="302" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A302">
+        <v>5</v>
+      </c>
+      <c r="B302" s="1">
+        <v>42739.532893518517</v>
+      </c>
+      <c r="C302">
+        <v>74244</v>
+      </c>
+      <c r="D302" t="s">
+        <v>595</v>
+      </c>
+      <c r="E302" t="s">
+        <v>1</v>
+      </c>
+      <c r="F302" s="2">
+        <v>0.13055555555555556</v>
+      </c>
+      <c r="G302" s="2">
+        <v>2.7083333333333334E-2</v>
+      </c>
+      <c r="H302" s="2">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="I302" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="303" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A303">
+        <v>6</v>
+      </c>
+      <c r="B303" s="1">
+        <v>42739.532395833332</v>
+      </c>
+      <c r="C303">
+        <v>56766</v>
+      </c>
+      <c r="D303" t="s">
+        <v>597</v>
+      </c>
+      <c r="E303" t="s">
+        <v>1</v>
+      </c>
+      <c r="F303" s="2">
+        <v>3.0555555555555555E-2</v>
+      </c>
+      <c r="G303" s="2">
+        <v>1.1805555555555555E-2</v>
+      </c>
+      <c r="H303" s="2">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="I303" t="s">
+        <v>598</v>
+      </c>
+    </row>
+    <row r="304" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A304">
+        <v>7</v>
+      </c>
+      <c r="B304" s="1">
+        <v>42739.532152777778</v>
+      </c>
+      <c r="C304">
+        <v>64653</v>
+      </c>
+      <c r="D304" t="s">
+        <v>599</v>
+      </c>
+      <c r="E304" t="s">
+        <v>1</v>
+      </c>
+      <c r="F304" s="2">
+        <v>4.9305555555555554E-2</v>
+      </c>
+      <c r="G304" s="2">
+        <v>2.013888888888889E-2</v>
+      </c>
+      <c r="H304" s="2">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="I304" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="305" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A305">
+        <v>8</v>
+      </c>
+      <c r="B305" s="1">
+        <v>42739.531215277777</v>
+      </c>
+      <c r="C305">
+        <v>57283</v>
+      </c>
+      <c r="D305" t="s">
+        <v>601</v>
+      </c>
+      <c r="E305" t="s">
+        <v>1</v>
+      </c>
+      <c r="F305" s="2">
+        <v>5.7638888888888885E-2</v>
+      </c>
+      <c r="G305" s="2">
+        <v>1.9444444444444445E-2</v>
+      </c>
+      <c r="H305" s="2">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="I305" t="s">
+        <v>602</v>
+      </c>
+    </row>
+    <row r="306" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A306">
+        <v>9</v>
+      </c>
+      <c r="B306" s="1">
+        <v>42739.530624999999</v>
+      </c>
+      <c r="C306">
+        <v>41039</v>
+      </c>
+      <c r="D306" t="s">
+        <v>603</v>
+      </c>
+      <c r="E306" t="s">
+        <v>1</v>
+      </c>
+      <c r="F306" s="2">
+        <v>5.0694444444444452E-2</v>
+      </c>
+      <c r="G306" s="2">
+        <v>1.3194444444444444E-2</v>
+      </c>
+      <c r="H306" s="2">
+        <v>4.8611111111111112E-3</v>
+      </c>
+      <c r="I306" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="307" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A307">
+        <v>10</v>
+      </c>
+      <c r="B307" s="1">
+        <v>42739.530347222222</v>
+      </c>
+      <c r="C307">
+        <v>148293</v>
+      </c>
+      <c r="D307" t="s">
+        <v>605</v>
+      </c>
+      <c r="E307" t="s">
+        <v>1</v>
+      </c>
+      <c r="F307" s="2">
+        <v>5.0694444444444452E-2</v>
+      </c>
+      <c r="G307" s="2">
+        <v>3.125E-2</v>
+      </c>
+      <c r="H307" s="2">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="I307" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="308" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A308">
+        <v>11</v>
+      </c>
+      <c r="B308" s="1">
+        <v>42739.529780092591</v>
+      </c>
+      <c r="C308">
+        <v>121602</v>
+      </c>
+      <c r="D308" t="s">
+        <v>607</v>
+      </c>
+      <c r="E308" t="s">
+        <v>1</v>
+      </c>
+      <c r="F308" s="2">
+        <v>4.9999999999999996E-2</v>
+      </c>
+      <c r="G308" s="2">
+        <v>9.8611111111111108E-2</v>
+      </c>
+      <c r="H308" s="2">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="I308" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="309" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A309">
+        <v>12</v>
+      </c>
+      <c r="B309" s="1">
+        <v>42739.528078703705</v>
+      </c>
+      <c r="C309">
+        <v>75472</v>
+      </c>
+      <c r="D309" t="s">
+        <v>609</v>
+      </c>
+      <c r="E309" t="s">
+        <v>1</v>
+      </c>
+      <c r="F309" s="2">
+        <v>6.458333333333334E-2</v>
+      </c>
+      <c r="G309" s="2">
+        <v>2.013888888888889E-2</v>
+      </c>
+      <c r="H309" s="2">
+        <v>4.8611111111111112E-3</v>
+      </c>
+      <c r="I309" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="310" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A310">
+        <v>1</v>
+      </c>
+      <c r="B310" s="1">
+        <v>42739.597870370373</v>
+      </c>
+      <c r="C310">
+        <v>120986</v>
+      </c>
+      <c r="D310" t="s">
+        <v>611</v>
+      </c>
+      <c r="E310" t="s">
+        <v>1</v>
+      </c>
+      <c r="F310" s="2">
+        <v>0.12361111111111112</v>
+      </c>
+      <c r="G310" s="2">
+        <v>3.1944444444444449E-2</v>
+      </c>
+      <c r="H310" s="2">
+        <v>0</v>
+      </c>
+      <c r="I310" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="311" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A311">
+        <v>2</v>
+      </c>
+      <c r="B311" s="1">
+        <v>42739.596886574072</v>
+      </c>
+      <c r="C311">
+        <v>106223</v>
+      </c>
+      <c r="D311" t="s">
+        <v>462</v>
+      </c>
+      <c r="E311" t="s">
+        <v>1</v>
+      </c>
+      <c r="F311" s="2">
+        <v>0.11041666666666666</v>
+      </c>
+      <c r="G311" s="2">
+        <v>7.9861111111111105E-2</v>
+      </c>
+      <c r="H311" s="2">
+        <v>5.2777777777777778E-2</v>
+      </c>
+      <c r="I311" t="s">
+        <v>613</v>
+      </c>
+    </row>
+    <row r="312" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A312">
+        <v>3</v>
+      </c>
+      <c r="B312" s="1">
+        <v>42739.592766203707</v>
+      </c>
+      <c r="C312">
+        <v>73537</v>
+      </c>
+      <c r="D312" t="s">
+        <v>614</v>
+      </c>
+      <c r="E312" t="s">
+        <v>1</v>
+      </c>
+      <c r="F312" s="2">
+        <v>7.9861111111111105E-2</v>
+      </c>
+      <c r="G312" s="2">
+        <v>5.0694444444444452E-2</v>
+      </c>
+      <c r="H312" s="2">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="I312" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="313" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A313">
+        <v>4</v>
+      </c>
+      <c r="B313" s="1">
+        <v>42739.591608796298</v>
+      </c>
+      <c r="C313">
+        <v>48419</v>
+      </c>
+      <c r="D313" t="s">
+        <v>616</v>
+      </c>
+      <c r="E313" t="s">
+        <v>1</v>
+      </c>
+      <c r="F313" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="G313" s="2">
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="H313" s="2">
+        <v>0</v>
+      </c>
+      <c r="I313" t="s">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="314" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A314">
+        <v>5</v>
+      </c>
+      <c r="B314" s="1">
+        <v>42739.591284722221</v>
+      </c>
+      <c r="C314">
+        <v>79017</v>
+      </c>
+      <c r="D314" t="s">
+        <v>618</v>
+      </c>
+      <c r="E314" t="s">
+        <v>1</v>
+      </c>
+      <c r="F314" s="2">
+        <v>6.1111111111111116E-2</v>
+      </c>
+      <c r="G314" s="2">
+        <v>1.5277777777777777E-2</v>
+      </c>
+      <c r="H314" s="2">
+        <v>4.1666666666666666E-3</v>
+      </c>
+      <c r="I314" t="s">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="315" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A315">
+        <v>6</v>
+      </c>
+      <c r="B315" s="1">
+        <v>42739.590254629627</v>
+      </c>
+      <c r="C315">
+        <v>168780</v>
+      </c>
+      <c r="D315" t="s">
+        <v>620</v>
+      </c>
+      <c r="E315" t="s">
+        <v>1</v>
+      </c>
+      <c r="F315" s="2">
+        <v>9.6527777777777768E-2</v>
+      </c>
+      <c r="G315" s="2">
+        <v>3.6111111111111115E-2</v>
+      </c>
+      <c r="H315" s="2">
+        <v>2.013888888888889E-2</v>
+      </c>
+      <c r="I315" t="s">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="316" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A316">
+        <v>7</v>
+      </c>
+      <c r="B316" s="1">
+        <v>42739.589583333334</v>
+      </c>
+      <c r="C316">
+        <v>4419</v>
+      </c>
+      <c r="D316" t="s">
+        <v>417</v>
+      </c>
+      <c r="E316" t="s">
+        <v>1</v>
+      </c>
+      <c r="F316" s="2">
+        <v>7.1527777777777787E-2</v>
+      </c>
+      <c r="G316" s="2">
+        <v>8.1250000000000003E-2</v>
+      </c>
+      <c r="H316" s="2">
+        <v>0</v>
+      </c>
+      <c r="I316" t="s">
+        <v>622</v>
+      </c>
+    </row>
+    <row r="317" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A317">
+        <v>8</v>
+      </c>
+      <c r="B317" s="1">
+        <v>42739.588043981479</v>
+      </c>
+      <c r="C317">
+        <v>63498</v>
+      </c>
+      <c r="D317" t="s">
+        <v>623</v>
+      </c>
+      <c r="E317" t="s">
+        <v>1</v>
+      </c>
+      <c r="F317" s="2">
+        <v>4.3750000000000004E-2</v>
+      </c>
+      <c r="G317" s="2">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="H317" s="2">
+        <v>0</v>
+      </c>
+      <c r="I317" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="318" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A318">
+        <v>9</v>
+      </c>
+      <c r="B318" s="1">
+        <v>42739.587881944448</v>
+      </c>
+      <c r="C318">
+        <v>111324</v>
+      </c>
+      <c r="D318" t="s">
+        <v>625</v>
+      </c>
+      <c r="E318" t="s">
+        <v>1</v>
+      </c>
+      <c r="F318" s="2">
+        <v>7.4305555555555555E-2</v>
+      </c>
+      <c r="G318" s="2">
+        <v>2.8472222222222222E-2</v>
+      </c>
+      <c r="H318" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="I318" t="s">
+        <v>626</v>
+      </c>
+    </row>
+    <row r="319" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A319">
+        <v>10</v>
+      </c>
+      <c r="B319" s="1">
+        <v>42739.587372685186</v>
+      </c>
+      <c r="C319">
+        <v>71417</v>
+      </c>
+      <c r="D319" t="s">
+        <v>627</v>
+      </c>
+      <c r="E319" t="s">
+        <v>1</v>
+      </c>
+      <c r="F319" s="2">
+        <v>5.486111111111111E-2</v>
+      </c>
+      <c r="G319" s="2">
+        <v>3.2638888888888891E-2</v>
+      </c>
+      <c r="H319" s="2">
+        <v>5.5555555555555558E-3</v>
+      </c>
+      <c r="I319" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="320" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A320">
+        <v>11</v>
+      </c>
+      <c r="B320" s="1">
+        <v>42739.586550925924</v>
+      </c>
+      <c r="C320">
+        <v>62315</v>
+      </c>
+      <c r="D320" t="s">
+        <v>629</v>
+      </c>
+      <c r="E320" t="s">
+        <v>1</v>
+      </c>
+      <c r="F320" s="2">
+        <v>4.0972222222222222E-2</v>
+      </c>
+      <c r="G320" s="2">
+        <v>2.1527777777777781E-2</v>
+      </c>
+      <c r="H320" s="2">
+        <v>0</v>
+      </c>
+      <c r="I320" t="s">
+        <v>630</v>
+      </c>
+    </row>
+    <row r="321" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A321">
+        <v>12</v>
+      </c>
+      <c r="B321" s="1">
+        <v>42739.586145833331</v>
+      </c>
+      <c r="C321">
+        <v>47210</v>
+      </c>
+      <c r="D321" t="s">
+        <v>631</v>
+      </c>
+      <c r="E321" t="s">
+        <v>1</v>
+      </c>
+      <c r="F321" s="2">
+        <v>3.888888888888889E-2</v>
+      </c>
+      <c r="G321" s="2">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="H321" s="2">
+        <v>0</v>
+      </c>
+      <c r="I321" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="322" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A322">
+        <v>13</v>
+      </c>
+      <c r="B322" s="1">
+        <v>42739.585868055554</v>
+      </c>
+      <c r="C322">
+        <v>88710</v>
+      </c>
+      <c r="D322" t="s">
+        <v>633</v>
+      </c>
+      <c r="E322" t="s">
+        <v>1</v>
+      </c>
+      <c r="F322" s="2">
+        <v>8.4027777777777771E-2</v>
+      </c>
+      <c r="G322" s="2">
+        <v>2.2222222222222223E-2</v>
+      </c>
+      <c r="H322" s="2">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="I322" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="323" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A323">
+        <v>14</v>
+      </c>
+      <c r="B323" s="1">
+        <v>42739.585439814815</v>
+      </c>
+      <c r="C323">
+        <v>78222</v>
+      </c>
+      <c r="D323" t="s">
+        <v>635</v>
+      </c>
+      <c r="E323" t="s">
+        <v>1</v>
+      </c>
+      <c r="F323" s="2">
+        <v>5.7638888888888885E-2</v>
+      </c>
+      <c r="G323" s="2">
+        <v>1.5277777777777777E-2</v>
+      </c>
+      <c r="H323" s="2">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="I323" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="324" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A324">
+        <v>15</v>
+      </c>
+      <c r="B324" s="1">
+        <v>42739.585034722222</v>
+      </c>
+      <c r="C324">
+        <v>169777</v>
+      </c>
+      <c r="D324" t="s">
+        <v>637</v>
+      </c>
+      <c r="E324" t="s">
+        <v>1</v>
+      </c>
+      <c r="F324" s="2">
+        <v>7.7777777777777779E-2</v>
+      </c>
+      <c r="G324" s="2">
+        <v>1.8055555555555557E-2</v>
+      </c>
+      <c r="H324" s="2">
+        <v>0</v>
+      </c>
+      <c r="I324" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="325" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A325">
+        <v>1</v>
+      </c>
+      <c r="B325" s="1">
+        <v>42739.661550925928</v>
+      </c>
+      <c r="C325">
+        <v>50391</v>
+      </c>
+      <c r="D325" t="s">
+        <v>639</v>
+      </c>
+      <c r="E325" t="s">
+        <v>1</v>
+      </c>
+      <c r="F325" s="2">
+        <v>3.9583333333333331E-2</v>
+      </c>
+      <c r="G325" s="2">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="H325" s="2">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="I325" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="326" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A326">
+        <v>2</v>
+      </c>
+      <c r="B326" s="1">
+        <v>42739.661261574074</v>
+      </c>
+      <c r="C326">
+        <v>48312</v>
+      </c>
+      <c r="D326" t="s">
+        <v>641</v>
+      </c>
+      <c r="E326" t="s">
+        <v>1</v>
+      </c>
+      <c r="F326" s="2">
+        <v>5.7638888888888885E-2</v>
+      </c>
+      <c r="G326" s="2">
+        <v>9.5833333333333326E-2</v>
+      </c>
+      <c r="H326" s="2">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="I326" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="327" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A327">
+        <v>3</v>
+      </c>
+      <c r="B327" s="1">
+        <v>42739.659629629627</v>
+      </c>
+      <c r="C327">
+        <v>176828</v>
+      </c>
+      <c r="D327" t="s">
+        <v>643</v>
+      </c>
+      <c r="E327" t="s">
+        <v>1</v>
+      </c>
+      <c r="F327" s="2">
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="G327" s="2">
+        <v>3.125E-2</v>
+      </c>
+      <c r="H327" s="2">
+        <v>9.0277777777777787E-3</v>
+      </c>
+      <c r="I327" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="328" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A328">
+        <v>4</v>
+      </c>
+      <c r="B328" s="1">
+        <v>42739.65898148148</v>
+      </c>
+      <c r="C328">
+        <v>43667</v>
+      </c>
+      <c r="D328" t="s">
+        <v>645</v>
+      </c>
+      <c r="E328" t="s">
+        <v>1</v>
+      </c>
+      <c r="F328" s="2">
+        <v>4.9999999999999996E-2</v>
+      </c>
+      <c r="G328" s="2">
+        <v>1.4583333333333332E-2</v>
+      </c>
+      <c r="H328" s="2">
+        <v>0</v>
+      </c>
+      <c r="I328" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="329" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A329">
+        <v>5</v>
+      </c>
+      <c r="B329" s="1">
+        <v>42739.658703703702</v>
+      </c>
+      <c r="C329">
+        <v>94860</v>
+      </c>
+      <c r="D329" t="s">
+        <v>647</v>
+      </c>
+      <c r="E329" t="s">
+        <v>1</v>
+      </c>
+      <c r="F329" s="2">
+        <v>4.7916666666666663E-2</v>
+      </c>
+      <c r="G329" s="2">
+        <v>7.4305555555555555E-2</v>
+      </c>
+      <c r="H329" s="2">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="I329" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="330" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A330">
+        <v>6</v>
+      </c>
+      <c r="B330" s="1">
+        <v>42739.65724537037</v>
+      </c>
+      <c r="C330">
+        <v>175824</v>
+      </c>
+      <c r="D330" t="s">
+        <v>649</v>
+      </c>
+      <c r="E330" t="s">
+        <v>1</v>
+      </c>
+      <c r="F330" s="2">
+        <v>4.5138888888888888E-2</v>
+      </c>
+      <c r="G330" s="2">
+        <v>3.888888888888889E-2</v>
+      </c>
+      <c r="H330" s="2">
+        <v>0</v>
+      </c>
+      <c r="I330" t="s">
+        <v>650</v>
+      </c>
+    </row>
+    <row r="331" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A331">
+        <v>7</v>
+      </c>
+      <c r="B331" s="1">
+        <v>42739.655902777777</v>
+      </c>
+      <c r="C331">
+        <v>164997</v>
+      </c>
+      <c r="D331" t="s">
+        <v>651</v>
+      </c>
+      <c r="E331" t="s">
+        <v>1</v>
+      </c>
+      <c r="F331" s="2">
+        <v>6.1805555555555558E-2</v>
+      </c>
+      <c r="G331" s="2">
+        <v>9.0277777777777776E-2</v>
+      </c>
+      <c r="H331" s="2">
+        <v>6.2499999999999995E-3</v>
+      </c>
+      <c r="I331" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="332" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A332">
+        <v>8</v>
+      </c>
+      <c r="B332" s="1">
+        <v>42739.654363425929</v>
+      </c>
+      <c r="C332">
+        <v>53873</v>
+      </c>
+      <c r="D332" t="s">
+        <v>653</v>
+      </c>
+      <c r="E332" t="s">
+        <v>1</v>
+      </c>
+      <c r="F332" s="2">
+        <v>5.9722222222222225E-2</v>
+      </c>
+      <c r="G332" s="2">
+        <v>1.8749999999999999E-2</v>
+      </c>
+      <c r="H332" s="2">
+        <v>0</v>
+      </c>
+      <c r="I332" t="s">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="333" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A333">
+        <v>9</v>
+      </c>
+      <c r="B333" s="1">
+        <v>42739.654004629629</v>
+      </c>
+      <c r="C333">
+        <v>23812</v>
+      </c>
+      <c r="D333" t="s">
+        <v>655</v>
+      </c>
+      <c r="E333" t="s">
+        <v>1</v>
+      </c>
+      <c r="F333" s="2">
+        <v>2.7777777777777776E-2</v>
+      </c>
+      <c r="G333" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="H333" s="2">
+        <v>0</v>
+      </c>
+      <c r="I333" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="334" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A334">
+        <v>10</v>
+      </c>
+      <c r="B334" s="1">
+        <v>42739.653599537036</v>
+      </c>
+      <c r="C334">
+        <v>149362</v>
+      </c>
+      <c r="D334" t="s">
+        <v>657</v>
+      </c>
+      <c r="E334" t="s">
+        <v>1</v>
+      </c>
+      <c r="F334" s="2">
+        <v>7.6388888888888895E-2</v>
+      </c>
+      <c r="G334" s="2">
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="H334" s="2">
+        <v>0</v>
+      </c>
+      <c r="I334" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="335" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A335">
+        <v>11</v>
+      </c>
+      <c r="B335" s="1">
+        <v>42739.653414351851</v>
+      </c>
+      <c r="C335">
+        <v>5440</v>
+      </c>
+      <c r="D335" t="s">
+        <v>659</v>
+      </c>
+      <c r="E335" t="s">
+        <v>1</v>
+      </c>
+      <c r="F335" s="2">
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="G335" s="2">
+        <v>2.6388888888888889E-2</v>
+      </c>
+      <c r="H335" s="2">
+        <v>0</v>
+      </c>
+      <c r="I335" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="336" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A336">
+        <v>1</v>
+      </c>
+      <c r="B336" s="1">
+        <v>42739.728854166664</v>
+      </c>
+      <c r="C336">
+        <v>57453</v>
+      </c>
+      <c r="D336" t="s">
+        <v>661</v>
+      </c>
+      <c r="E336" t="s">
+        <v>1</v>
+      </c>
+      <c r="F336" s="2">
+        <v>6.3194444444444442E-2</v>
+      </c>
+      <c r="G336" s="2">
+        <v>6.1111111111111116E-2</v>
+      </c>
+      <c r="H336" s="2">
+        <v>4.8611111111111112E-3</v>
+      </c>
+      <c r="I336" t="s">
+        <v>662</v>
+      </c>
+    </row>
+    <row r="337" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A337">
+        <v>2</v>
+      </c>
+      <c r="B337" s="1">
+        <v>42739.727754629632</v>
+      </c>
+      <c r="C337">
+        <v>106256</v>
+      </c>
+      <c r="D337" t="s">
+        <v>663</v>
+      </c>
+      <c r="E337" t="s">
+        <v>1</v>
+      </c>
+      <c r="F337" s="2">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="G337" s="2">
+        <v>1.8055555555555557E-2</v>
+      </c>
+      <c r="H337" s="2">
+        <v>0</v>
+      </c>
+      <c r="I337" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="338" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A338">
+        <v>3</v>
+      </c>
+      <c r="B338" s="1">
+        <v>42739.727395833332</v>
+      </c>
+      <c r="C338">
+        <v>79370</v>
+      </c>
+      <c r="D338" t="s">
+        <v>665</v>
+      </c>
+      <c r="E338" t="s">
+        <v>1</v>
+      </c>
+      <c r="F338" s="2">
+        <v>0.11875000000000001</v>
+      </c>
+      <c r="G338" s="2">
+        <v>7.3611111111111113E-2</v>
+      </c>
+      <c r="H338" s="2">
+        <v>8.3333333333333332E-3</v>
+      </c>
+      <c r="I338" t="s">
+        <v>666</v>
+      </c>
+    </row>
+    <row r="339" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A339">
+        <v>4</v>
+      </c>
+      <c r="B339" s="1">
+        <v>42739.725752314815</v>
+      </c>
+      <c r="C339">
+        <v>93983</v>
+      </c>
+      <c r="D339" t="s">
+        <v>667</v>
+      </c>
+      <c r="E339" t="s">
+        <v>1</v>
+      </c>
+      <c r="F339" s="2">
+        <v>4.8611111111111112E-2</v>
+      </c>
+      <c r="G339" s="2">
+        <v>3.8194444444444441E-2</v>
+      </c>
+      <c r="H339" s="2">
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="I339" t="s">
+        <v>668</v>
+      </c>
+    </row>
+    <row r="340" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A340">
+        <v>5</v>
+      </c>
+      <c r="B340" s="1">
+        <v>42739.725023148145</v>
+      </c>
+      <c r="C340">
+        <v>130760</v>
+      </c>
+      <c r="D340" t="s">
+        <v>669</v>
+      </c>
+      <c r="E340" t="s">
+        <v>1</v>
+      </c>
+      <c r="F340" s="2">
+        <v>0.1076388888888889</v>
+      </c>
+      <c r="G340" s="2">
+        <v>4.2361111111111106E-2</v>
+      </c>
+      <c r="H340" s="2">
+        <v>4.1666666666666666E-3</v>
+      </c>
+      <c r="I340" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="341" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A341">
+        <v>6</v>
+      </c>
+      <c r="B341" s="1">
+        <v>42739.723101851851</v>
+      </c>
+      <c r="C341">
+        <v>75383</v>
+      </c>
+      <c r="D341" t="s">
+        <v>671</v>
+      </c>
+      <c r="E341" t="s">
+        <v>1</v>
+      </c>
+      <c r="F341" s="2">
+        <v>7.1527777777777787E-2</v>
+      </c>
+      <c r="G341" s="2">
+        <v>0.15277777777777776</v>
+      </c>
+      <c r="H341" s="2">
+        <v>7.013888888888889E-2</v>
+      </c>
+      <c r="I341" t="s">
+        <v>672</v>
+      </c>
+    </row>
+    <row r="342" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A342">
+        <v>7</v>
+      </c>
+      <c r="B342" s="1">
+        <v>42739.719884259262</v>
+      </c>
+      <c r="C342">
+        <v>102986</v>
+      </c>
+      <c r="D342" t="s">
+        <v>673</v>
+      </c>
+      <c r="E342" t="s">
+        <v>1</v>
+      </c>
+      <c r="F342" s="2">
+        <v>7.8472222222222221E-2</v>
+      </c>
+      <c r="G342" s="2">
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="H342" s="2">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="I342" t="s">
+        <v>674</v>
+      </c>
+    </row>
+    <row r="343" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A343">
+        <v>8</v>
+      </c>
+      <c r="B343" s="1">
+        <v>42739.719571759262</v>
+      </c>
+      <c r="C343">
+        <v>104096</v>
+      </c>
+      <c r="D343" t="s">
+        <v>675</v>
+      </c>
+      <c r="E343" t="s">
+        <v>1</v>
+      </c>
+      <c r="F343" s="2">
+        <v>8.8888888888888892E-2</v>
+      </c>
+      <c r="G343" s="2">
+        <v>8.819444444444445E-2</v>
+      </c>
+      <c r="H343" s="2">
+        <v>6.2499999999999995E-3</v>
+      </c>
+      <c r="I343" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="344" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A344">
+        <v>9</v>
+      </c>
+      <c r="B344" s="1">
+        <v>42739.718055555553</v>
+      </c>
+      <c r="C344">
+        <v>166402</v>
+      </c>
+      <c r="D344" t="s">
+        <v>677</v>
+      </c>
+      <c r="E344" t="s">
+        <v>1</v>
+      </c>
+      <c r="F344" s="2">
+        <v>4.2361111111111106E-2</v>
+      </c>
+      <c r="G344" s="2">
+        <v>1.2499999999999999E-2</v>
+      </c>
+      <c r="H344" s="2">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="I344" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="345" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A345">
+        <v>10</v>
+      </c>
+      <c r="B345" s="1">
+        <v>42739.717812499999</v>
+      </c>
+      <c r="C345">
+        <v>62628</v>
+      </c>
+      <c r="D345" t="s">
+        <v>679</v>
+      </c>
+      <c r="E345" t="s">
+        <v>1</v>
+      </c>
+      <c r="F345" s="2">
+        <v>4.3750000000000004E-2</v>
+      </c>
+      <c r="G345" s="2">
+        <v>1.6666666666666666E-2</v>
+      </c>
+      <c r="H345" s="2">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="I345" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="346" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A346">
+        <v>11</v>
+      </c>
+      <c r="B346" s="1">
+        <v>42739.717453703706</v>
+      </c>
+      <c r="C346">
+        <v>103770</v>
+      </c>
+      <c r="D346" t="s">
+        <v>681</v>
+      </c>
+      <c r="E346" t="s">
+        <v>1</v>
+      </c>
+      <c r="F346" s="2">
+        <v>3.6111111111111115E-2</v>
+      </c>
+      <c r="G346" s="2">
+        <v>1.9444444444444445E-2</v>
+      </c>
+      <c r="H346" s="2">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="I346" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="347" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A347">
+        <v>12</v>
+      </c>
+      <c r="B347" s="1">
+        <v>42739.71707175926</v>
+      </c>
+      <c r="C347">
+        <v>52783</v>
+      </c>
+      <c r="D347" t="s">
+        <v>192</v>
+      </c>
+      <c r="E347" t="s">
+        <v>1</v>
+      </c>
+      <c r="F347" s="2">
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="G347" s="2">
+        <v>2.2222222222222223E-2</v>
+      </c>
+      <c r="H347" s="2">
+        <v>7.6388888888888886E-3</v>
+      </c>
+      <c r="I347" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="348" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A348">
+        <v>13</v>
+      </c>
+      <c r="B348" s="1">
+        <v>42739.716458333336</v>
+      </c>
+      <c r="C348">
+        <v>45843</v>
+      </c>
+      <c r="D348" t="s">
+        <v>684</v>
+      </c>
+      <c r="E348" t="s">
+        <v>1</v>
+      </c>
+      <c r="F348" s="2">
+        <v>7.4305555555555555E-2</v>
+      </c>
+      <c r="G348" s="2">
+        <v>0.18194444444444444</v>
+      </c>
+      <c r="H348" s="2">
+        <v>0</v>
+      </c>
+      <c r="I348" t="s">
+        <v>685</v>
+      </c>
+    </row>
+    <row r="349" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A349">
+        <v>14</v>
+      </c>
+      <c r="B349" s="1">
+        <v>42739.713391203702</v>
+      </c>
+      <c r="C349">
+        <v>56619</v>
+      </c>
+      <c r="D349" t="s">
+        <v>686</v>
+      </c>
+      <c r="E349" t="s">
+        <v>1</v>
+      </c>
+      <c r="F349" s="2">
+        <v>3.125E-2</v>
+      </c>
+      <c r="G349" s="2">
+        <v>1.5972222222222224E-2</v>
+      </c>
+      <c r="H349" s="2">
+        <v>0</v>
+      </c>
+      <c r="I349" t="s">
+        <v>687</v>
+      </c>
+    </row>
+    <row r="350" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A350">
+        <v>15</v>
+      </c>
+      <c r="B350" s="1">
+        <v>42739.71292824074</v>
+      </c>
+      <c r="C350">
+        <v>97763</v>
+      </c>
+      <c r="D350" t="s">
+        <v>688</v>
+      </c>
+      <c r="E350" t="s">
+        <v>1</v>
+      </c>
+      <c r="F350" s="2">
+        <v>3.6111111111111115E-2</v>
+      </c>
+      <c r="G350" s="2">
+        <v>5.5555555555555558E-3</v>
+      </c>
+      <c r="H350" s="2">
+        <v>0</v>
+      </c>
+      <c r="I350" t="s">
+        <v>689</v>
+      </c>
+    </row>
+    <row r="351" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A351">
+        <v>16</v>
+      </c>
+      <c r="B351" s="1">
+        <v>42739.712777777779</v>
+      </c>
+      <c r="C351">
+        <v>99656</v>
+      </c>
+      <c r="D351" t="s">
+        <v>690</v>
+      </c>
+      <c r="E351" t="s">
+        <v>1</v>
+      </c>
+      <c r="F351" s="2">
+        <v>2.9166666666666664E-2</v>
+      </c>
+      <c r="G351" s="2">
+        <v>1.3888888888888888E-2</v>
+      </c>
+      <c r="H351" s="2">
+        <v>0</v>
+      </c>
+      <c r="I351" t="s">
+        <v>691</v>
+      </c>
+    </row>
+    <row r="352" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A352">
+        <v>17</v>
+      </c>
+      <c r="B352" s="1">
+        <v>42739.712500000001</v>
+      </c>
+      <c r="C352">
+        <v>32120</v>
+      </c>
+      <c r="D352" t="s">
+        <v>692</v>
+      </c>
+      <c r="E352" t="s">
+        <v>1</v>
+      </c>
+      <c r="F352" s="2">
+        <v>6.25E-2</v>
+      </c>
+      <c r="G352" s="2">
+        <v>2.9166666666666664E-2</v>
+      </c>
+      <c r="H352" s="2">
+        <v>1.3194444444444444E-2</v>
+      </c>
+      <c r="I352" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="353" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A353">
+        <v>18</v>
+      </c>
+      <c r="B353" s="1">
+        <v>42739.711967592593</v>
+      </c>
+      <c r="C353">
+        <v>174515</v>
+      </c>
+      <c r="D353" t="s">
+        <v>552</v>
+      </c>
+      <c r="E353" t="s">
+        <v>1</v>
+      </c>
+      <c r="F353" s="2">
+        <v>5.2777777777777778E-2</v>
+      </c>
+      <c r="G353" s="2">
+        <v>2.9166666666666664E-2</v>
+      </c>
+      <c r="H353" s="2">
+        <v>1.3194444444444444E-2</v>
+      </c>
+      <c r="I353" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="354" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A354">
+        <v>19</v>
+      </c>
+      <c r="B354" s="1">
+        <v>42739.711261574077</v>
+      </c>
+      <c r="C354">
+        <v>162601</v>
+      </c>
+      <c r="D354" t="s">
+        <v>695</v>
+      </c>
+      <c r="E354" t="s">
+        <v>1</v>
+      </c>
+      <c r="F354" s="2">
+        <v>6.0416666666666667E-2</v>
+      </c>
+      <c r="G354" s="2">
+        <v>2.9861111111111113E-2</v>
+      </c>
+      <c r="H354" s="2">
+        <v>0</v>
+      </c>
+      <c r="I354" t="s">
+        <v>696</v>
+      </c>
+    </row>
+    <row r="355" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A355">
+        <v>20</v>
+      </c>
+      <c r="B355" s="1">
+        <v>42739.710555555554</v>
+      </c>
+      <c r="C355">
+        <v>157029</v>
+      </c>
+      <c r="D355" t="s">
+        <v>697</v>
+      </c>
+      <c r="E355" t="s">
+        <v>1</v>
+      </c>
+      <c r="F355" s="2">
+        <v>7.5694444444444439E-2</v>
+      </c>
+      <c r="G355" s="2">
+        <v>3.4722222222222224E-2</v>
+      </c>
+      <c r="H355" s="2">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="I355" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="356" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A356">
+        <v>21</v>
+      </c>
+      <c r="B356" s="1">
+        <v>42739.709930555553</v>
+      </c>
+      <c r="C356">
+        <v>52858</v>
+      </c>
+      <c r="D356" t="s">
+        <v>699</v>
+      </c>
+      <c r="E356" t="s">
+        <v>1</v>
+      </c>
+      <c r="F356" s="2">
+        <v>6.5972222222222224E-2</v>
+      </c>
+      <c r="G356" s="2">
+        <v>1.4583333333333332E-2</v>
+      </c>
+      <c r="H356" s="2">
+        <v>6.9444444444444447E-4</v>
+      </c>
+      <c r="I356" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="357" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A357">
+        <v>22</v>
+      </c>
+      <c r="B357" s="1">
+        <v>42739.709629629629</v>
+      </c>
+      <c r="C357">
+        <v>71349</v>
+      </c>
+      <c r="D357" t="s">
+        <v>224</v>
+      </c>
+      <c r="E357" t="s">
+        <v>1</v>
+      </c>
+      <c r="F357" s="2">
+        <v>8.1944444444444445E-2</v>
+      </c>
+      <c r="G357" s="2">
+        <v>5.4166666666666669E-2</v>
+      </c>
+      <c r="H357" s="2">
+        <v>2.0833333333333333E-3</v>
+      </c>
+      <c r="I357" t="s">
+        <v>701</v>
+      </c>
+    </row>
+    <row r="358" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A358">
+        <v>23</v>
+      </c>
+      <c r="B358" s="1">
+        <v>42739.708645833336</v>
+      </c>
+      <c r="C358">
+        <v>177225</v>
+      </c>
+      <c r="D358" t="s">
+        <v>702</v>
+      </c>
+      <c r="E358" t="s">
+        <v>1</v>
+      </c>
+      <c r="F358" s="2">
+        <v>8.5416666666666655E-2</v>
+      </c>
+      <c r="G358" s="2">
+        <v>0.13819444444444443</v>
+      </c>
+      <c r="H358" s="2">
+        <v>5.5555555555555558E-3</v>
+      </c>
+      <c r="I358" t="s">
+        <v>703</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>